<commit_message>
correction bug upload file*
</commit_message>
<xml_diff>
--- a/database/test.xlsx
+++ b/database/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xtian\OneDrive\Documents\CentralSupelec\projet\msdocs-flask-postgresql-sample-app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F474B50-06DF-40BD-83A4-308C57F65A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F6AEBD-5731-4C03-83A7-44182AF52C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="3120" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J70" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X107"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,7 +1590,7 @@
         <v>0.14513192999999999</v>
       </c>
       <c r="X2" s="6">
-        <v>9999</v>
+        <v>9996</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Ajout de la fonction de maj journaliere de produits manquants
</commit_message>
<xml_diff>
--- a/database/test.xlsx
+++ b/database/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xtian\OneDrive\Documents\CentralSupelec\projet\msdocs-flask-postgresql-sample-app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF2CA14-9C53-41A2-BFF0-E17BD6247BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1F4F7-8E59-43C8-AAFE-89DB2C063779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1420,7 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
@@ -1590,7 +1590,7 @@
         <v>0.14513192999999999</v>
       </c>
       <c r="X2" s="6">
-        <v>99998</v>
+        <v>99991</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>6</v>

</xml_diff>